<commit_message>
saved audio assets excel file
</commit_message>
<xml_diff>
--- a/Audio/Audio Assets.xlsx
+++ b/Audio/Audio Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarkusAuer\Repositories\xrcc_kickup\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92E04B6-A56B-4869-BC27-F69E6167484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E7BA0E-F4F0-4F4F-AD79-7E271389D5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" xr2:uid="{FF038C4D-D925-4DEE-8AC8-D7A64C8FB6AB}"/>
+    <workbookView xWindow="2976" yWindow="1824" windowWidth="23040" windowHeight="13560" xr2:uid="{FF038C4D-D925-4DEE-8AC8-D7A64C8FB6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Pencil-Palooza</t>
   </si>
@@ -80,13 +80,16 @@
     <t>SFX_Ingame_Pencil_draw_loop_02</t>
   </si>
   <si>
-    <t>SFX_Ingame_Pencil_draw_loop_03</t>
-  </si>
-  <si>
     <t>Audio Assets List</t>
   </si>
   <si>
     <t>Asset name</t>
+  </si>
+  <si>
+    <t>exported</t>
+  </si>
+  <si>
+    <t>✅</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,7 +511,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -519,19 +522,19 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -542,65 +545,85 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
+      <c r="C10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sound gui button click game start
</commit_message>
<xml_diff>
--- a/Audio/Audio Assets.xlsx
+++ b/Audio/Audio Assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarkusAuer\Repositories\xrcc_kickup\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E7BA0E-F4F0-4F4F-AD79-7E271389D5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF39401-3818-4444-83D2-55A8BD32B300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2976" yWindow="1824" windowWidth="23040" windowHeight="13560" xr2:uid="{FF038C4D-D925-4DEE-8AC8-D7A64C8FB6AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Pencil-Palooza</t>
   </si>
@@ -53,12 +53,6 @@
     <t>SFX_Ingame_Card_popup</t>
   </si>
   <si>
-    <t>GUI_Button_Hover</t>
-  </si>
-  <si>
-    <t>GUI_Button_Select</t>
-  </si>
-  <si>
     <t>SFX_Ingame_Char_</t>
   </si>
   <si>
@@ -90,6 +84,18 @@
   </si>
   <si>
     <t>✅</t>
+  </si>
+  <si>
+    <t>GUI_Button_Menu_Hover</t>
+  </si>
+  <si>
+    <t>GUI_Button_Menu_Select</t>
+  </si>
+  <si>
+    <t>GUI_Button_StartGame_Hover</t>
+  </si>
+  <si>
+    <t>GUI_Button_StartGame_Select</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609CBCC3-2DEE-4B1B-93DC-3634A6AE9009}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -511,7 +517,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -522,108 +528,121 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>